<commit_message>
Added evolution of indices vs NFE and updated metrics study
</commit_message>
<xml_diff>
--- a/matlab/metrics_strudy_results.xlsx
+++ b/matlab/metrics_strudy_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20377"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SEAK Lab\SEAK Lab Github\VASSAR\VASSAR_exec_heur\matlab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosha\Documents\SEAK Lab Github\VASSAR\VASSAR_exec_heur\matlab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411099F6-1265-4715-9AD0-18F106948547}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D45468F-FFFF-4BE0-967C-08A21F0B01D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17280" windowHeight="12228" firstSheet="7" activeTab="8" xr2:uid="{B3241343-5121-41A6-AFB4-A8CC1D2CC9E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="9" activeTab="11" xr2:uid="{B3241343-5121-41A6-AFB4-A8CC1D2CC9E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Random Designs (incorrect)" sheetId="1" r:id="rId1"/>
@@ -22,18 +22,32 @@
     <sheet name="Random + GA Designs EOSS-AIAA" sheetId="7" r:id="rId7"/>
     <sheet name="Random + GA vassarheur_assign" sheetId="8" r:id="rId8"/>
     <sheet name="Random + GA vassarheur_partitio" sheetId="9" r:id="rId9"/>
+    <sheet name="Assigning journal" sheetId="10" r:id="rId10"/>
+    <sheet name="Partitioning journal" sheetId="11" r:id="rId11"/>
+    <sheet name="Assigning journal2" sheetId="12" r:id="rId12"/>
+    <sheet name="Partitioning journal2" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2462" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2622" uniqueCount="150">
   <si>
     <t>Category</t>
   </si>
@@ -597,6 +611,12 @@
   </si>
   <si>
     <t>Spearman’s Coefficient p-value</t>
+  </si>
+  <si>
+    <t>Support values - Random</t>
+  </si>
+  <si>
+    <t>Support values - Random + GA</t>
   </si>
 </sst>
 </file>
@@ -4705,6 +4725,1754 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D30DF960-FA24-4BA7-BF9D-E25F8612833F}">
+  <dimension ref="C4:G40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="3:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+    </row>
+    <row r="9" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="33">
+        <v>8.6666666666666697E-3</v>
+      </c>
+      <c r="E9" s="33">
+        <v>4.7661356865615996E-3</v>
+      </c>
+      <c r="F9" s="34"/>
+      <c r="G9" s="33"/>
+    </row>
+    <row r="10" spans="3:7" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+    </row>
+    <row r="11" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1.66666666666667E-3</v>
+      </c>
+      <c r="E11" s="33">
+        <v>1.7568209223157701E-3</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.998</v>
+      </c>
+      <c r="E12" s="33">
+        <v>3.2203059435976498E-3</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row r="14" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="17" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" spans="3:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="33">
+        <v>8.6499999999999994E-2</v>
+      </c>
+      <c r="E21" s="33">
+        <v>1.2433775188256301E-2</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row r="22" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="33">
+        <v>2.33333333333333E-2</v>
+      </c>
+      <c r="E22" s="33">
+        <v>1.6759003476664799E-2</v>
+      </c>
+      <c r="F22" s="34">
+        <v>0.20312041063484301</v>
+      </c>
+      <c r="G22" s="33">
+        <v>7.9975262340006195E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="33">
+        <v>3.1333333333333303E-2</v>
+      </c>
+      <c r="E23" s="33">
+        <v>2.5175924223230201E-2</v>
+      </c>
+      <c r="F23" s="33">
+        <v>3.00013888888888E-2</v>
+      </c>
+      <c r="G23" s="33">
+        <v>2.2574359819119798E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0.24283333333333301</v>
+      </c>
+      <c r="E24" s="33">
+        <v>5.8304490223711897E-2</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0.65253194444444496</v>
+      </c>
+      <c r="G24" s="33">
+        <v>0.46982613064979301</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0.97933333333333294</v>
+      </c>
+      <c r="E25" s="33">
+        <v>1.75365579347126E-2</v>
+      </c>
+      <c r="F25" s="33">
+        <v>1.694957368308E-3</v>
+      </c>
+      <c r="G25" s="33">
+        <v>1.1966627538269299E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0.120833333333333</v>
+      </c>
+      <c r="E26" s="33">
+        <v>2.2100360312128999E-2</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0.16689861642815801</v>
+      </c>
+      <c r="G26" s="33">
+        <v>0.11621451553395699</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="33">
+        <v>1.83333333333333E-3</v>
+      </c>
+      <c r="E27" s="33">
+        <v>5.7975090436420303E-3</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0.63547694444444403</v>
+      </c>
+      <c r="G27" s="33">
+        <v>0.42868435084807199</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C30" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="3:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="55"/>
+      <c r="F33" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="55"/>
+    </row>
+    <row r="34" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="22"/>
+      <c r="D34" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="21">
+        <v>0.18514707350196799</v>
+      </c>
+      <c r="E35" s="21">
+        <v>0.144357022449418</v>
+      </c>
+      <c r="F35" s="21">
+        <v>0.158201578248238</v>
+      </c>
+      <c r="G35" s="21">
+        <v>0.14438080838741199</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="21">
+        <v>0.87648793868156105</v>
+      </c>
+      <c r="E36" s="21">
+        <v>2.4920231085698099E-2</v>
+      </c>
+      <c r="F36" s="21">
+        <v>0.81022043548071498</v>
+      </c>
+      <c r="G36" s="21">
+        <v>2.1298527362252202E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="21">
+        <v>0.74170957338394605</v>
+      </c>
+      <c r="E37" s="21">
+        <v>3.7922790199193097E-2</v>
+      </c>
+      <c r="F37" s="21">
+        <v>0.74118881632217404</v>
+      </c>
+      <c r="G37" s="21">
+        <v>2.8176196185708002E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="21">
+        <v>-0.109852095325745</v>
+      </c>
+      <c r="E38" s="21">
+        <v>5.6462052681988797E-2</v>
+      </c>
+      <c r="F38" s="21">
+        <v>-8.9027564815895494E-2</v>
+      </c>
+      <c r="G38" s="21">
+        <v>5.0562458533266602E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="21">
+        <v>0.76958896674926003</v>
+      </c>
+      <c r="E39" s="21">
+        <v>3.7491268617457801E-2</v>
+      </c>
+      <c r="F39" s="21">
+        <v>0.76143146849424703</v>
+      </c>
+      <c r="G39" s="21">
+        <v>4.0934943400502397E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="21">
+        <v>0.83054523103923295</v>
+      </c>
+      <c r="E40" s="21">
+        <v>4.0307252409297299E-2</v>
+      </c>
+      <c r="F40" s="21">
+        <v>0.78112994746502895</v>
+      </c>
+      <c r="G40" s="21">
+        <v>2.93774920323971E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95703F01-4AE7-47B5-BBAA-CDAFF5BCB380}">
+  <dimension ref="C5:G41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:G41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C5" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+    </row>
+    <row r="8" spans="3:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="3:7" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+    </row>
+    <row r="10" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="33">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E10" s="33">
+        <v>1.47572957474524E-2</v>
+      </c>
+      <c r="F10" s="34"/>
+      <c r="G10" s="33"/>
+    </row>
+    <row r="11" spans="3:7" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="33">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="E11" s="33">
+        <v>1.10888666221108E-2</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="33">
+        <v>5.6666666666666698E-2</v>
+      </c>
+      <c r="E12" s="33">
+        <v>1.1653431646335E-2</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="E13" s="33">
+        <v>1.7458946555127999E-2</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row r="14" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0.42966666666666697</v>
+      </c>
+      <c r="E14" s="33">
+        <v>3.0609044092341602E-2</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="15" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C15" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="33">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0</v>
+      </c>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+    </row>
+    <row r="18" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+    </row>
+    <row r="21" spans="3:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="33">
+        <v>1.3333333333333299E-2</v>
+      </c>
+      <c r="E22" s="33">
+        <v>2.6057865332352399E-3</v>
+      </c>
+      <c r="F22" s="33"/>
+      <c r="G22" s="33"/>
+    </row>
+    <row r="23" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="33">
+        <v>0.10716666666666699</v>
+      </c>
+      <c r="E23" s="33">
+        <v>7.2665519868626696E-2</v>
+      </c>
+      <c r="F23" s="34">
+        <v>3.3823782416723597E-2</v>
+      </c>
+      <c r="G23" s="33">
+        <v>7.1533867871793305E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0.421833333333333</v>
+      </c>
+      <c r="E24" s="33">
+        <v>5.4299409996112498E-2</v>
+      </c>
+      <c r="F24" s="33">
+        <v>1.18234795040351E-2</v>
+      </c>
+      <c r="G24" s="33">
+        <v>2.0496177900883299E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0.52833333333333299</v>
+      </c>
+      <c r="E25" s="33">
+        <v>5.8267158231675199E-3</v>
+      </c>
+      <c r="F25" s="33">
+        <v>0.20314968013468099</v>
+      </c>
+      <c r="G25" s="33">
+        <v>0.27479315177847002</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" s="33">
+        <v>0.95150000000000001</v>
+      </c>
+      <c r="E26" s="33">
+        <v>8.7294732775639698E-3</v>
+      </c>
+      <c r="F26" s="33">
+        <v>1.91285358924772E-3</v>
+      </c>
+      <c r="G26" s="33">
+        <v>9.8506816139240904E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="33">
+        <v>0.71483333333333299</v>
+      </c>
+      <c r="E27" s="33">
+        <v>1.5304522046170801E-2</v>
+      </c>
+      <c r="F27" s="33">
+        <v>2.71327948146327E-2</v>
+      </c>
+      <c r="G27" s="33">
+        <v>7.8087885533697304E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C28" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="33">
+        <v>8.3333333333333297E-3</v>
+      </c>
+      <c r="E28" s="33">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33">
+        <v>0.26831691317941497</v>
+      </c>
+      <c r="G28" s="33">
+        <v>9.8245471644719695E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C31" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="34" spans="3:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D34" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="55"/>
+      <c r="F34" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="55"/>
+    </row>
+    <row r="35" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="22"/>
+      <c r="D35" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D36" s="21">
+        <v>0.44324592148331399</v>
+      </c>
+      <c r="E36" s="21">
+        <v>2.0200986462015801E-2</v>
+      </c>
+      <c r="F36" s="21">
+        <v>0.71473174499216796</v>
+      </c>
+      <c r="G36" s="21">
+        <v>7.7459628034372202E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="21">
+        <v>0.65517073633233303</v>
+      </c>
+      <c r="E37" s="21">
+        <v>1.05309213500094E-2</v>
+      </c>
+      <c r="F37" s="21">
+        <v>0.84976686923563505</v>
+      </c>
+      <c r="G37" s="21">
+        <v>6.7217323008930602E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D38" s="21">
+        <v>0.70534667482486002</v>
+      </c>
+      <c r="E38" s="21">
+        <v>1.7651379878475201E-2</v>
+      </c>
+      <c r="F38" s="21">
+        <v>0.79840519329325998</v>
+      </c>
+      <c r="G38" s="21">
+        <v>2.1095693641717001E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D39" s="21">
+        <v>0.197564125693412</v>
+      </c>
+      <c r="E39" s="21">
+        <v>2.3658415443828198E-2</v>
+      </c>
+      <c r="F39" s="21">
+        <v>0.214146770714531</v>
+      </c>
+      <c r="G39" s="21">
+        <v>2.2791836278225099E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="21">
+        <v>0.3783892751106</v>
+      </c>
+      <c r="E40" s="21">
+        <v>2.67768731825632E-2</v>
+      </c>
+      <c r="F40" s="21">
+        <v>0.60711969352151096</v>
+      </c>
+      <c r="G40" s="21">
+        <v>2.41055732245847E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C41" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D41" s="21">
+        <v>0.46760506617875702</v>
+      </c>
+      <c r="E41" s="21">
+        <v>5.4566188609265001E-2</v>
+      </c>
+      <c r="F41" s="21">
+        <v>0.53631519236217196</v>
+      </c>
+      <c r="G41" s="21">
+        <v>0.126456883841218</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="F34:G34"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AD7B112-1F2C-4F6E-A22A-B918C94FAE5E}">
+  <dimension ref="C4:G40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C4" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+    </row>
+    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C5" s="29"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+    </row>
+    <row r="6" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+    </row>
+    <row r="7" spans="3:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C7" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:7" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+    </row>
+    <row r="9" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="33">
+        <v>8.6666666666666697E-3</v>
+      </c>
+      <c r="E9" s="33">
+        <v>4.7661356865615996E-3</v>
+      </c>
+      <c r="F9" s="34"/>
+      <c r="G9" s="33"/>
+    </row>
+    <row r="10" spans="3:7" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+    </row>
+    <row r="11" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="33">
+        <v>1.66666666666667E-3</v>
+      </c>
+      <c r="E11" s="33">
+        <v>1.7568209223157701E-3</v>
+      </c>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+    </row>
+    <row r="12" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0.998</v>
+      </c>
+      <c r="E12" s="33">
+        <v>3.2203059435976498E-3</v>
+      </c>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+    </row>
+    <row r="13" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="33">
+        <v>0</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0</v>
+      </c>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+    </row>
+    <row r="14" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="33">
+        <v>0</v>
+      </c>
+      <c r="E14" s="33">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+    </row>
+    <row r="17" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+    </row>
+    <row r="19" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+    </row>
+    <row r="20" spans="3:7" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C20" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C21" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="33">
+        <v>4.4333333333333301E-2</v>
+      </c>
+      <c r="E21" s="33">
+        <v>4.9190985824841497E-3</v>
+      </c>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+    </row>
+    <row r="22" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C22" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="33">
+        <v>1.38333333333333E-2</v>
+      </c>
+      <c r="E22" s="33">
+        <v>8.2794554601162904E-3</v>
+      </c>
+      <c r="F22" s="34">
+        <v>0.207906840446896</v>
+      </c>
+      <c r="G22" s="33">
+        <v>8.4911838914046106E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C23" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="33">
+        <v>5.6666666666666697E-3</v>
+      </c>
+      <c r="E23" s="33">
+        <v>4.5946829173634102E-3</v>
+      </c>
+      <c r="F23" s="33">
+        <v>3.9020910493827297E-2</v>
+      </c>
+      <c r="G23" s="33">
+        <v>1.8939799825269402E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="33">
+        <v>0.105</v>
+      </c>
+      <c r="E24" s="33">
+        <v>5.6234737298331401E-2</v>
+      </c>
+      <c r="F24" s="33">
+        <v>0.786892777777778</v>
+      </c>
+      <c r="G24" s="33">
+        <v>0.41916152098916798</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="33">
+        <v>0.97283333333333299</v>
+      </c>
+      <c r="E25" s="33">
+        <v>1.8971225775036401E-2</v>
+      </c>
+      <c r="F25" s="33">
+        <v>1.76570907444026E-3</v>
+      </c>
+      <c r="G25" s="33">
+        <v>1.1744954337183099E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="D26" s="33">
+        <v>3.11666666666667E-2</v>
+      </c>
+      <c r="E26" s="33">
+        <v>1.1195512769535799E-2</v>
+      </c>
+      <c r="F26" s="33">
+        <v>0.19795330091101501</v>
+      </c>
+      <c r="G26" s="33">
+        <v>0.10441632919051901</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C27" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="33">
+        <v>1.6666666666666701E-4</v>
+      </c>
+      <c r="E27" s="33">
+        <v>5.2704627669473004E-4</v>
+      </c>
+      <c r="F27" s="33">
+        <v>0.79399138888888898</v>
+      </c>
+      <c r="G27" s="33">
+        <v>0.366130392027402</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="C30" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="3:7" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C33" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="E33" s="55"/>
+      <c r="F33" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="55"/>
+    </row>
+    <row r="34" spans="3:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C34" s="22"/>
+      <c r="D34" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C35" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="21">
+        <v>0.131326318440076</v>
+      </c>
+      <c r="E35" s="21">
+        <v>0.107172893612349</v>
+      </c>
+      <c r="F35" s="21">
+        <v>0.113033231425637</v>
+      </c>
+      <c r="G35" s="21">
+        <v>0.123285855641832</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C36" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="21">
+        <v>0.75076014314974004</v>
+      </c>
+      <c r="E36" s="21">
+        <v>6.0114839945044102E-2</v>
+      </c>
+      <c r="F36" s="21">
+        <v>0.72139071870711002</v>
+      </c>
+      <c r="G36" s="21">
+        <v>5.07413042223415E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C37" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D37" s="21">
+        <v>0.630416465284383</v>
+      </c>
+      <c r="E37" s="21">
+        <v>7.4245353502644301E-2</v>
+      </c>
+      <c r="F37" s="21">
+        <v>0.61339415079256199</v>
+      </c>
+      <c r="G37" s="21">
+        <v>7.1218793534455399E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C38" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D38" s="21">
+        <v>-0.15350800886695801</v>
+      </c>
+      <c r="E38" s="21">
+        <v>4.7767519247349302E-2</v>
+      </c>
+      <c r="F38" s="21">
+        <v>-0.16186564710696</v>
+      </c>
+      <c r="G38" s="21">
+        <v>5.18262444901951E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C39" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D39" s="21">
+        <v>0.67217052043735703</v>
+      </c>
+      <c r="E39" s="21">
+        <v>6.9848773748229204E-2</v>
+      </c>
+      <c r="F39" s="21">
+        <v>0.66438508190883305</v>
+      </c>
+      <c r="G39" s="21">
+        <v>7.0633024841490505E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C40" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D40" s="21">
+        <v>0.682159780647009</v>
+      </c>
+      <c r="E40" s="21">
+        <v>7.3844596409901403E-2</v>
+      </c>
+      <c r="F40" s="21">
+        <v>0.66243760762803205</v>
+      </c>
+      <c r="G40" s="21">
+        <v>6.4289810784112597E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="F33:G33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F36222C6-70E7-40E2-89C9-E2AA33F18721}">
+  <dimension ref="D4:H40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="L39" sqref="L39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="4:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D4" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+    </row>
+    <row r="6" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+    </row>
+    <row r="7" spans="4:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D7" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D8" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+    </row>
+    <row r="9" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D9" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="33">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="F9" s="33">
+        <v>1.47572957474524E-2</v>
+      </c>
+      <c r="G9" s="34"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="4:8" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D10" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="33">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F10" s="33">
+        <v>1.10888666221108E-2</v>
+      </c>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+    </row>
+    <row r="11" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="33">
+        <v>5.6666666666666698E-2</v>
+      </c>
+      <c r="F11" s="33">
+        <v>1.1653431646335E-2</v>
+      </c>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0.90300000000000002</v>
+      </c>
+      <c r="F12" s="33">
+        <v>1.7458946555127999E-2</v>
+      </c>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+    </row>
+    <row r="13" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="33">
+        <v>0.42966666666666697</v>
+      </c>
+      <c r="F13" s="33">
+        <v>3.0609044092341602E-2</v>
+      </c>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+    </row>
+    <row r="14" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="33">
+        <v>1.6666666666666701E-2</v>
+      </c>
+      <c r="F14" s="34">
+        <v>0</v>
+      </c>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+    </row>
+    <row r="17" spans="4:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D17" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D18" s="29"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="29"/>
+    </row>
+    <row r="19" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="29"/>
+    </row>
+    <row r="20" spans="4:8" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="31" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" s="31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F20" s="31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="H20" s="31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" ht="24.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="33">
+        <v>1.0833333333333301E-2</v>
+      </c>
+      <c r="F21" s="33">
+        <v>2.9658550700087001E-3</v>
+      </c>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+    </row>
+    <row r="22" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E22" s="33">
+        <v>8.7333333333333402E-2</v>
+      </c>
+      <c r="F22" s="33">
+        <v>4.7695018763124701E-2</v>
+      </c>
+      <c r="G22" s="34">
+        <v>5.3048425401428297E-2</v>
+      </c>
+      <c r="H22" s="33">
+        <v>8.2118430336844406E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" ht="60.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="32" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" s="33">
+        <v>0.203666666666667</v>
+      </c>
+      <c r="F23" s="33">
+        <v>3.34239509009207E-2</v>
+      </c>
+      <c r="G23" s="33">
+        <v>1.6591630591630699E-2</v>
+      </c>
+      <c r="H23" s="33">
+        <v>2.1363273745912601E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D24" s="32" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="33">
+        <v>0.211666666666667</v>
+      </c>
+      <c r="F24" s="33">
+        <v>3.7646831880216503E-2</v>
+      </c>
+      <c r="G24" s="33">
+        <v>0.334523569023571</v>
+      </c>
+      <c r="H24" s="33">
+        <v>0.28695172240203798</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="32" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="33">
+        <v>0.91649999999999998</v>
+      </c>
+      <c r="F25" s="33">
+        <v>1.13705814915857E-2</v>
+      </c>
+      <c r="G25" s="33">
+        <v>3.2663273872305999E-3</v>
+      </c>
+      <c r="H25" s="33">
+        <v>1.2652845550963601E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D26" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="33">
+        <v>0.53166666666666695</v>
+      </c>
+      <c r="F26" s="33">
+        <v>2.61524495465329E-2</v>
+      </c>
+      <c r="G26" s="33">
+        <v>4.2031373886956498E-2</v>
+      </c>
+      <c r="H26" s="33">
+        <v>9.0519389691772006E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="33">
+        <v>1.16666666666667E-2</v>
+      </c>
+      <c r="F27" s="34">
+        <v>1.82855909821703E-18</v>
+      </c>
+      <c r="G27" s="33">
+        <v>0.29668965127465102</v>
+      </c>
+      <c r="H27" s="33">
+        <v>0.110637650522111</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="D30" s="28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="33" spans="4:8" ht="55.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="55"/>
+      <c r="G33" s="54" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="55"/>
+    </row>
+    <row r="34" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="22"/>
+      <c r="E34" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="37" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="H34" s="37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="4:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D35" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" s="21">
+        <v>0.24931817877430901</v>
+      </c>
+      <c r="F35" s="21">
+        <v>5.2746180884775201E-2</v>
+      </c>
+      <c r="G35" s="21">
+        <v>0.40486961528658699</v>
+      </c>
+      <c r="H35" s="21">
+        <v>9.0356883459121198E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="4:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="E36" s="21">
+        <v>0.58816882196651199</v>
+      </c>
+      <c r="F36" s="21">
+        <v>5.52444598687441E-2</v>
+      </c>
+      <c r="G36" s="21">
+        <v>0.79328558415772099</v>
+      </c>
+      <c r="H36" s="21">
+        <v>6.0485178524461503E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="4:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="E37" s="21">
+        <v>0.403508297725159</v>
+      </c>
+      <c r="F37" s="21">
+        <v>6.4833740890466798E-2</v>
+      </c>
+      <c r="G37" s="21">
+        <v>0.43839732230054401</v>
+      </c>
+      <c r="H37" s="21">
+        <v>7.6852207307786399E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="4:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="E38" s="21">
+        <v>9.8017560422760205E-2</v>
+      </c>
+      <c r="F38" s="21">
+        <v>4.9046770173782499E-2</v>
+      </c>
+      <c r="G38" s="21">
+        <v>0.101912382496282</v>
+      </c>
+      <c r="H38" s="21">
+        <v>6.2334943201483597E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E39" s="21">
+        <v>0.249417676828289</v>
+      </c>
+      <c r="F39" s="21">
+        <v>5.0236225363007703E-2</v>
+      </c>
+      <c r="G39" s="21">
+        <v>0.36918709094755298</v>
+      </c>
+      <c r="H39" s="21">
+        <v>6.6841440045220996E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D40" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E40" s="21">
+        <v>0.27869233721925002</v>
+      </c>
+      <c r="F40" s="21">
+        <v>5.5658710693009601E-2</v>
+      </c>
+      <c r="G40" s="21">
+        <v>0.315056366330561</v>
+      </c>
+      <c r="H40" s="21">
+        <v>7.2497805002150403E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:H33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{834C2348-B346-4E72-834E-AC1969B49FB8}">
   <dimension ref="B6:U154"/>
@@ -25565,8 +27333,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D210A2E1-7160-4BCA-8393-B00F59F1697C}">
   <dimension ref="B6:U154"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L32" sqref="L32"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F41" sqref="B34:F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -29161,7 +30929,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122C9584-0EFD-432A-8614-6F95393DA6AE}">
   <dimension ref="B6:U154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>

</xml_diff>